<commit_message>
V3 Gerbers and STEP Files
</commit_message>
<xml_diff>
--- a/PCB Design/.PCBsV3/FlyBoxBoard.xlsx
+++ b/PCB Design/.PCBsV3/FlyBoxBoard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obradley\OneDrive - Olin College of Engineering\Documents\GitHub\FlyBox\PCB Design\.PCBsV2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obradley\OneDrive - Olin College of Engineering\Documents\GitHub\FlyBox\PCB Design\.PCBsV3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F42871-EEE3-45BA-8C7B-1CF889469BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA47A2E-5D15-4D85-9958-64F0D70CD832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,9 +154,6 @@
     <t>4 Pin 5.08 screw terminal</t>
   </si>
   <si>
-    <t>T-1V8W547848A BOM</t>
-  </si>
-  <si>
     <t>5V in,
 12V in, 
 RED, 
@@ -270,6 +267,9 @@
 Potentiometer,
 GND,
 ESP 32 unused pins,</t>
+  </si>
+  <si>
+    <t>T-1D14W547848A BOM</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1240,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,7 +1255,7 @@
       <c r="B1" s="17"/>
       <c r="C1" s="1"/>
       <c r="D1" s="18" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
@@ -1319,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -1328,7 +1328,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -1345,7 +1345,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1354,7 +1354,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -1371,25 +1371,25 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1397,19 +1397,19 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="F9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" t="s">
         <v>17</v>
@@ -1420,7 +1420,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1432,7 +1432,7 @@
         <v>61301011821</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
         <v>17</v>
@@ -1443,7 +1443,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -1455,7 +1455,7 @@
         <v>61300511821</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" t="s">
         <v>17</v>
@@ -1478,7 +1478,7 @@
         <v>61300611821</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" t="s">
         <v>17</v>
@@ -1501,7 +1501,7 @@
         <v>62000211821</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
@@ -1512,7 +1512,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1524,7 +1524,7 @@
         <v>61300311821</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" t="s">
         <v>17</v>
@@ -1535,19 +1535,19 @@
         <v>9</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -1558,25 +1558,25 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>8</v>
       </c>
       <c r="D16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="F16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="G16" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -1587,13 +1587,13 @@
         <v>1</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="16">
         <v>1729157</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s">
         <v>17</v>
@@ -1610,13 +1610,13 @@
         <v>1</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="16">
         <v>1729160</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H18" t="s">
         <v>17</v>

</xml_diff>